<commit_message>
Added M0 and M1 to tasks sheet. Populated/updated M0
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="M-1 Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="M-0.5" sheetId="4" r:id="rId2"/>
-    <sheet name="Links" sheetId="2" r:id="rId3"/>
-    <sheet name="Notes" sheetId="3" r:id="rId4"/>
+    <sheet name="M0 - Account Mgmt" sheetId="5" r:id="rId3"/>
+    <sheet name="M1 - Game Data" sheetId="6" r:id="rId4"/>
+    <sheet name="Links" sheetId="2" r:id="rId5"/>
+    <sheet name="Notes" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="97">
   <si>
     <t>Status</t>
   </si>
@@ -226,6 +228,99 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Change Admin password</t>
+  </si>
+  <si>
+    <t>Change User password</t>
+  </si>
+  <si>
+    <t>Delete User account</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>Change Avatar</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>View User Profile</t>
+  </si>
+  <si>
+    <t>View Users List</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
+  <si>
+    <t>ADMIN FEATURES</t>
+  </si>
+  <si>
+    <t>USER FEATURES</t>
+  </si>
+  <si>
+    <t>Allow OAUTH2 Logins from Facebook</t>
+  </si>
+  <si>
+    <t>Allow OAUTH2 Logins from Google</t>
+  </si>
+  <si>
+    <t>Modify/Update user model to include missing fields</t>
+  </si>
+  <si>
+    <t>Add any missing/required fields from model to registration page</t>
+  </si>
+  <si>
+    <t>Admin Controller</t>
+  </si>
+  <si>
+    <t>User Controller</t>
+  </si>
+  <si>
+    <t>Login/Auth</t>
+  </si>
+  <si>
+    <t>User Model</t>
+  </si>
+  <si>
+    <t>Registration View</t>
+  </si>
+  <si>
+    <t>Add default avatars to database</t>
+  </si>
+  <si>
+    <t>Create Admin View (and model/controller if required)</t>
+  </si>
+  <si>
+    <t>Promote User to Admin</t>
+  </si>
+  <si>
+    <t>See StartupAuth.cs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May need future updates to support faction avatar. </t>
+  </si>
+  <si>
+    <t>Obscure/encrypt connection string ID/Password</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Connection string is in Web.Config</t>
+  </si>
+  <si>
+    <t>Fix code-first migrations on server</t>
   </si>
 </sst>
 </file>
@@ -937,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,6 +1201,314 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.75" customWidth="1"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="72.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64.875" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="94.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
@@ -1185,7 +1588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added standard legal text file to docs. Updated tasks sheet.
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
   <si>
     <t>Status</t>
   </si>
@@ -341,20 +341,26 @@
     <t>In progress</t>
   </si>
   <si>
-    <t xml:space="preserve">Initial setup done; Controllers/View need refining, and role access needs setting. </t>
-  </si>
-  <si>
-    <t>name still in user; faction removed (will become avatar icon), UserGame missing faction icon.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Probably already have this, but look at it carefully. Make sure both user an admin can do it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logos live on webserver and are loaded based on a path string derived from a stored faction db entry. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started, but needs further work. DELAYED. PART OF M1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User model has avatar field; UserGame doesn't need a faction; GameLog entries will derive a faction logo from the army for that game entry. </t>
+  </si>
+  <si>
+    <t>NEXT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,8 +405,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,8 +461,13 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -449,14 +475,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -468,10 +510,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1232,7 +1277,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1285,7 @@
     <col min="1" max="1" width="54.75" customWidth="1"/>
     <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="73.125" customWidth="1"/>
+    <col min="4" max="4" width="129.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1264,6 +1309,9 @@
       <c r="B2" t="s">
         <v>83</v>
       </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1283,8 +1331,11 @@
       <c r="B4" t="s">
         <v>83</v>
       </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,6 +1345,9 @@
       <c r="B5" t="s">
         <v>83</v>
       </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1302,6 +1356,9 @@
       <c r="B6" t="s">
         <v>83</v>
       </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1406,11 +1463,11 @@
       <c r="B17" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>104</v>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,11 +1477,11 @@
       <c r="B18" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>103</v>
+      <c r="D18" s="10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1492,6 +1549,12 @@
       <c r="A25" t="s">
         <v>88</v>
       </c>
+      <c r="C25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1514,6 +1577,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
reminder note added to task list
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
   <si>
     <t>Status</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>NEXT</t>
+  </si>
+  <si>
+    <t>Reminder: Move jquery scripts to a .js file and remove from register view</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,6 +1576,14 @@
       </c>
       <c r="C27" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added admin menu page, Users contoller
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="115">
   <si>
     <t>Status</t>
   </si>
@@ -341,9 +341,6 @@
     <t>In progress</t>
   </si>
   <si>
-    <t xml:space="preserve">Probably already have this, but look at it carefully. Make sure both user an admin can do it. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Logos live on webserver and are loaded based on a path string derived from a stored faction db entry. </t>
   </si>
   <si>
@@ -357,6 +354,27 @@
   </si>
   <si>
     <t>Reminder: Move jquery scripts to a .js file and remove from register view</t>
+  </si>
+  <si>
+    <t>Create Admin Game controller</t>
+  </si>
+  <si>
+    <t>Game Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can edit the hash, but don't have a way to manually reset the password. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin view created and restricted by role. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modify Users list to display their roles (admin, TO, etc.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requires a new ViewModel. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create additional viewmodel first. </t>
   </si>
 </sst>
 </file>
@@ -1277,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,8 +1330,11 @@
       <c r="B2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
-        <v>107</v>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1332,13 +1353,10 @@
         <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>103</v>
+        <v>84</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,10 +1364,10 @@
         <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
+        <v>84</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,51 +1378,54 @@
         <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>84</v>
@@ -1415,7 +1436,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
@@ -1426,23 +1447,29 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
       </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>84</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
         <v>84</v>
@@ -1450,139 +1477,155 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>99</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="D20" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added User ViewModel that includes user roles for Users/Index
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="113">
   <si>
     <t>Status</t>
   </si>
@@ -362,19 +362,13 @@
     <t>Game Controller</t>
   </si>
   <si>
-    <t xml:space="preserve">Can edit the hash, but don't have a way to manually reset the password. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Admin view created and restricted by role. </t>
   </si>
   <si>
     <t xml:space="preserve">Modify Users list to display their roles (admin, TO, etc.) </t>
   </si>
   <si>
-    <t xml:space="preserve">Requires a new ViewModel. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create additional viewmodel first. </t>
+    <t>Users can't request a forgotten password. Need this as a workaround, or need to configure password reset request.</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1292,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1328,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,7 +1350,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1380,9 +1374,6 @@
       <c r="C6" t="s">
         <v>106</v>
       </c>
-      <c r="D6" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1397,16 +1388,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="C8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" t="s">
-        <v>113</v>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
User Promotions controller and view added. (No func. yet).
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
   <si>
     <t>Status</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Create Admin View (and model/controller if required)</t>
   </si>
   <si>
-    <t>Promote User to Admin</t>
-  </si>
-  <si>
     <t>See StartupAuth.cs</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>Security</t>
   </si>
   <si>
-    <t>Connection string is in Web.Config</t>
-  </si>
-  <si>
     <t>Fix code-first migrations on server</t>
   </si>
   <si>
@@ -350,9 +344,6 @@
     <t xml:space="preserve">User model has avatar field; UserGame doesn't need a faction; GameLog entries will derive a faction logo from the army for that game entry. </t>
   </si>
   <si>
-    <t>NEXT</t>
-  </si>
-  <si>
     <t>Reminder: Move jquery scripts to a .js file and remove from register view</t>
   </si>
   <si>
@@ -368,7 +359,46 @@
     <t xml:space="preserve">Modify Users list to display their roles (admin, TO, etc.) </t>
   </si>
   <si>
-    <t>Users can't request a forgotten password. Need this as a workaround, or need to configure password reset request.</t>
+    <t>Promote User to Admin or Organizer</t>
+  </si>
+  <si>
+    <t>Implement "Forgot Password"</t>
+  </si>
+  <si>
+    <t>User password</t>
+  </si>
+  <si>
+    <t>Connection string is in Web.Config --&gt; If this is the only place it shows up it should be safe, as nobody should have access to the sourcecode. (if they do it's too late)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Think about how to store/retrieve score summary data. </t>
+  </si>
+  <si>
+    <t>Show User name, avatar image on index after login</t>
+  </si>
+  <si>
+    <t>Home Controller</t>
+  </si>
+  <si>
+    <t>Create new home view for logged-in users. (Right now we're just duplicating the main index)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Better solution: implement forgot password reset request. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in content for legal page and hook up the link properly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal view. </t>
+  </si>
+  <si>
+    <t>Remove User From Role</t>
+  </si>
+  <si>
+    <t>Need to add controller POST and connect to View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to add controller POST and connect to View. </t>
   </si>
 </sst>
 </file>
@@ -1289,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,7 +1358,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,7 +1380,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,65 +1396,71 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
-        <v>106</v>
+      <c r="C6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>83</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
@@ -1435,7 +1471,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
@@ -1446,7 +1482,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
         <v>84</v>
@@ -1457,15 +1493,18 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>84</v>
       </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>84</v>
@@ -1473,7 +1512,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
         <v>84</v>
@@ -1481,140 +1520,178 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Users Controller: renamed 'Promote' to 'Roles'. Added POST action and cleaned up form
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="121">
   <si>
     <t>Status</t>
   </si>
@@ -368,12 +368,6 @@
     <t>User password</t>
   </si>
   <si>
-    <t>Connection string is in Web.Config --&gt; If this is the only place it shows up it should be safe, as nobody should have access to the sourcecode. (if they do it's too late)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Think about how to store/retrieve score summary data. </t>
-  </si>
-  <si>
     <t>Show User name, avatar image on index after login</t>
   </si>
   <si>
@@ -395,10 +389,10 @@
     <t>Remove User From Role</t>
   </si>
   <si>
-    <t>Need to add controller POST and connect to View</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to add controller POST and connect to View. </t>
+    <t xml:space="preserve">Connection string is in Web.Config --&gt; Will show up on github. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. </t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1316,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1374,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,25 +1395,19 @@
       <c r="B6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>121</v>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>122</v>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1526,7 +1514,7 @@
         <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,13 +1558,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" t="s">
         <v>114</v>
-      </c>
-      <c r="B22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,7 +1647,7 @@
         <v>93</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1688,10 +1676,10 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new Main screen separate from Index; Worked with avatar img displays
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
   <si>
     <t>Status</t>
   </si>
@@ -374,9 +374,6 @@
     <t>Home Controller</t>
   </si>
   <si>
-    <t>Create new home view for logged-in users. (Right now we're just duplicating the main index)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Better solution: implement forgot password reset request. </t>
   </si>
   <si>
@@ -393,6 +390,30 @@
   </si>
   <si>
     <t xml:space="preserve">Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. </t>
+  </si>
+  <si>
+    <t>In progress.</t>
+  </si>
+  <si>
+    <t>New view created. Need to add buttons/links. (Subscribe to game, log game entry)</t>
+  </si>
+  <si>
+    <t>User Partial View for insertion on multiple pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show Avatar, Name, e-mail … </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Admin/Users so that it displays the user avatars </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do this in a way that it can be easily recycled on other pages. </t>
+  </si>
+  <si>
+    <t>Users, Global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show avatar setting on the account management page. </t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1395,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,7 +1422,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -1497,6 +1518,9 @@
       <c r="B16" t="s">
         <v>84</v>
       </c>
+      <c r="D16" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1514,7 +1538,7 @@
         <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,38 +1587,39 @@
       <c r="B22" t="s">
         <v>113</v>
       </c>
+      <c r="C22" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="D22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>85</v>
@@ -1605,81 +1630,103 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D29" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>18</v>
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>110</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
         <v>116</v>
       </c>
-      <c r="B34" t="s">
-        <v>117</v>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting user session vars on login; Created global helpers class
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="128">
   <si>
     <t>Status</t>
   </si>
@@ -1337,7 +1337,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D36" sqref="A35:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1598,6 @@
       <c r="A23" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="5"/>
       <c r="D23" t="s">
         <v>123</v>
       </c>
@@ -1700,6 +1699,9 @@
       </c>
       <c r="B33" t="s">
         <v>87</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
UserInfoBox partial view added; hooked up legal screen
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="128">
   <si>
     <t>Status</t>
   </si>
@@ -329,9 +329,6 @@
     <t>UserGame Controller</t>
   </si>
   <si>
-    <t xml:space="preserve">Requires some design. End goal is to support multiple games. Easier to do now rather than later. </t>
-  </si>
-  <si>
     <t>In progress</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
     <t xml:space="preserve">Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. </t>
   </si>
   <si>
-    <t>In progress.</t>
-  </si>
-  <si>
     <t>New view created. Need to add buttons/links. (Subscribe to game, log game entry)</t>
   </si>
   <si>
@@ -414,6 +408,12 @@
   </si>
   <si>
     <t xml:space="preserve">Show avatar setting on the account management page. </t>
+  </si>
+  <si>
+    <t>Requires some design. End goal is to support multiple games. Easier to do now rather than later.  Should give it a better than than UserGames. E.g. GameLogs</t>
+  </si>
+  <si>
+    <t>NEXT</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1337,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="A35:D36"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1373,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,7 +1411,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -1433,10 +1433,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>18</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
         <v>84</v>
@@ -1453,34 +1453,37 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
@@ -1491,7 +1494,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
         <v>84</v>
@@ -1502,7 +1505,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
         <v>84</v>
@@ -1513,123 +1516,126 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
         <v>84</v>
       </c>
-      <c r="D16" t="s">
-        <v>127</v>
+      <c r="C16" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
         <v>84</v>
       </c>
+      <c r="D17" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>84</v>
       </c>
-      <c r="D18" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" t="s">
-        <v>121</v>
+        <v>98</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
         <v>85</v>
@@ -1640,95 +1646,98 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>87</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D30" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>92</v>
-      </c>
-      <c r="B31" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C33" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" t="s">
         <v>110</v>
       </c>
-      <c r="B34" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" t="s">
-        <v>126</v>
-      </c>
-      <c r="D36" t="s">
-        <v>125</v>
+      <c r="C36" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added custom Html.Image helper class for displaying avatars and icons
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
   <si>
     <t>Status</t>
   </si>
@@ -383,9 +383,6 @@
     <t>Remove User From Role</t>
   </si>
   <si>
-    <t xml:space="preserve">Connection string is in Web.Config --&gt; Will show up on github. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. </t>
   </si>
   <si>
@@ -401,9 +398,6 @@
     <t xml:space="preserve">Change Admin/Users so that it displays the user avatars </t>
   </si>
   <si>
-    <t xml:space="preserve">Do this in a way that it can be easily recycled on other pages. </t>
-  </si>
-  <si>
     <t>Users, Global</t>
   </si>
   <si>
@@ -413,7 +407,10 @@
     <t>Requires some design. End goal is to support multiple games. Easier to do now rather than later.  Should give it a better than than UserGames. E.g. GameLogs</t>
   </si>
   <si>
-    <t>NEXT</t>
+    <t>Connection string is in Web.Config --&gt; Will show up on github.  See this for solution: http://stackoverflow.com/questions/5630352/avoiding-asp-net-passwords-in-github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactored this to use a custom Html Helper for images. </t>
   </si>
 </sst>
 </file>
@@ -898,10 +895,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.25" customWidth="1"/>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="70.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1170,10 +1167,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.25" customWidth="1"/>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="70.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,16 +1333,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.75" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="129.125" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="143.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1455,16 +1452,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
         <v>122</v>
       </c>
-      <c r="B10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>127</v>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1533,7 +1530,7 @@
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,7 +1549,7 @@
         <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,7 +1560,7 @@
         <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,18 +1602,18 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>120</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1699,7 +1696,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1756,10 +1753,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.875" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="94.125" customWidth="1"/>
+    <col min="1" max="1" width="64.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="94.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1819,8 +1816,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="92.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1899,7 +1896,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.625" customWidth="1"/>
+    <col min="1" max="1" width="90.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix avatar display after update; Removed Stored Session variables
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="130">
   <si>
     <t>Status</t>
   </si>
@@ -404,13 +404,22 @@
     <t xml:space="preserve">Show avatar setting on the account management page. </t>
   </si>
   <si>
-    <t>Requires some design. End goal is to support multiple games. Easier to do now rather than later.  Should give it a better than than UserGames. E.g. GameLogs</t>
-  </si>
-  <si>
     <t>Connection string is in Web.Config --&gt; Will show up on github.  See this for solution: http://stackoverflow.com/questions/5630352/avoiding-asp-net-passwords-in-github</t>
   </si>
   <si>
     <t xml:space="preserve">Refactored this to use a custom Html Helper for images. </t>
+  </si>
+  <si>
+    <t>NEXT</t>
+  </si>
+  <si>
+    <t>Requires some design. End goal is to support multiple games. Easier to do now rather than later.  Should give it a better name than UserGames. E.g. GameLogs</t>
+  </si>
+  <si>
+    <t>REVISIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ties to item below. </t>
   </si>
 </sst>
 </file>
@@ -1331,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,7 +1470,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,48 +1531,64 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
       <c r="B17" t="s">
         <v>84</v>
       </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="D17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>75</v>
       </c>
       <c r="B19" t="s">
         <v>84</v>
       </c>
+      <c r="C19" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="D19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -1577,7 +1602,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -1591,7 +1616,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>111</v>
       </c>
@@ -1605,7 +1630,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -1616,7 +1641,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
@@ -1630,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1641,7 +1666,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -1652,7 +1677,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -1666,7 +1691,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -1677,7 +1702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1688,7 +1713,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -1696,7 +1721,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rename Games to SupportedGames; Db Migration
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Code\CSharp\StatsMachine\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\CSharp\StatsMachine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -383,9 +383,6 @@
     <t>Remove User From Role</t>
   </si>
   <si>
-    <t xml:space="preserve">Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. </t>
-  </si>
-  <si>
     <t>New view created. Need to add buttons/links. (Subscribe to game, log game entry)</t>
   </si>
   <si>
@@ -413,20 +410,23 @@
     <t>NEXT</t>
   </si>
   <si>
-    <t>Requires some design. End goal is to support multiple games. Easier to do now rather than later.  Should give it a better name than UserGames. E.g. GameLogs</t>
-  </si>
-  <si>
     <t>REVISIT</t>
   </si>
   <si>
     <t xml:space="preserve">Ties to item below. </t>
+  </si>
+  <si>
+    <t>Requires some design. End goal is to support multiple games. Need to think about how to bind SupportedGames -&gt; UserGames -&gt; Games.{Title}.  ( or SG -&gt; UG -&gt; G -&gt; GameDetails</t>
+  </si>
+  <si>
+    <t>Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. -&gt; Viewmodel UsersByGame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,14 +472,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -577,7 +569,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="4"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -904,10 +896,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.25" customWidth="1"/>
+    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="3" max="3" width="16.25" customWidth="1"/>
+    <col min="4" max="4" width="70.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1176,10 +1168,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.25" customWidth="1"/>
+    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="3" max="3" width="16.25" customWidth="1"/>
+    <col min="4" max="4" width="70.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,16 +1334,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="143.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.75" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="143.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1461,16 +1453,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
         <v>121</v>
       </c>
-      <c r="B10" t="s">
-        <v>122</v>
-      </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1542,7 +1534,7 @@
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1553,10 +1545,10 @@
         <v>84</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,10 +1559,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1581,10 +1573,10 @@
         <v>86</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="E20" s="8"/>
     </row>
@@ -1627,18 +1619,18 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>119</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1721,7 +1713,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1764,7 +1756,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1778,10 +1770,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="94.140625" customWidth="1"/>
+    <col min="1" max="1" width="64.875" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="94.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,8 +1833,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="92.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1921,7 +1913,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.5703125" customWidth="1"/>
+    <col min="1" max="1" width="90.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactor: changed SupportedGames to GameSystems
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\CSharp\StatsMachine\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Code\CSharp\StatsMachine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -416,10 +416,10 @@
     <t xml:space="preserve">Ties to item below. </t>
   </si>
   <si>
-    <t>Requires some design. End goal is to support multiple games. Need to think about how to bind SupportedGames -&gt; UserGames -&gt; Games.{Title}.  ( or SG -&gt; UG -&gt; G -&gt; GameDetails</t>
-  </si>
-  <si>
     <t>Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. -&gt; Viewmodel UsersByGame</t>
+  </si>
+  <si>
+    <t>Refactor: table = GameSystem. GameId  becomes the string name; Update User_Game models and controllers with the changes. Game tables will use the game name</t>
   </si>
 </sst>
 </file>
@@ -896,10 +896,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.25" customWidth="1"/>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="70.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,10 +1168,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.25" customWidth="1"/>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="70.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1335,15 +1335,15 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.75" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="143.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="155" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>126</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E20" s="8"/>
     </row>
@@ -1770,10 +1770,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.875" customWidth="1"/>
-    <col min="2" max="2" width="18.375" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="94.125" customWidth="1"/>
+    <col min="1" max="1" width="64.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="94.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1833,8 +1833,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="92.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.625" customWidth="1"/>
+    <col min="1" max="1" width="90.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Removed all CRUD functions from GameSystem; Started UserGame admin view
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Code\CSharp\StatsMachine\Docs\"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="132">
   <si>
     <t>Status</t>
   </si>
@@ -413,13 +413,19 @@
     <t>REVISIT</t>
   </si>
   <si>
-    <t xml:space="preserve">Ties to item below. </t>
-  </si>
-  <si>
     <t>Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. -&gt; Viewmodel UsersByGame</t>
   </si>
   <si>
-    <t>Refactor: table = GameSystem. GameId  becomes the string name; Update User_Game models and controllers with the changes. Game tables will use the game name</t>
+    <t xml:space="preserve">MANUALLY CREATE WARMACHINE TABLE w/ Schema. Update database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin -&gt; User Games -&gt; Needs fixing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to hook up code to properly link a userid with a gameid. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ties to item below. Note: Should also be able to show all games subscribed -&gt; Will require a view model. </t>
   </si>
 </sst>
 </file>
@@ -1332,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1554,7 @@
         <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1562,7 +1568,7 @@
         <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,7 +1582,7 @@
         <v>126</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20" s="8"/>
     </row>
@@ -1716,7 +1722,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -1752,6 +1758,16 @@
       </c>
       <c r="C36" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring of UserGames m/v/c; Added Warmachine model
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="130">
   <si>
     <t>Status</t>
   </si>
@@ -416,16 +416,10 @@
     <t>Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. -&gt; Viewmodel UsersByGame</t>
   </si>
   <si>
-    <t xml:space="preserve">MANUALLY CREATE WARMACHINE TABLE w/ Schema. Update database. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin -&gt; User Games -&gt; Needs fixing. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to hook up code to properly link a userid with a gameid. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ties to item below. Note: Should also be able to show all games subscribed -&gt; Will require a view model. </t>
+  </si>
+  <si>
+    <t>Change the UserGame table to use the userid, and update the controllers. Then create viewmodel that shows the e-mail rather than the userid, and update the views.</t>
   </si>
 </sst>
 </file>
@@ -562,7 +556,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -576,6 +570,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1340,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -1554,7 +1551,7 @@
         <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1579,7 @@
         <v>126</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E20" s="8"/>
     </row>
@@ -1761,14 +1758,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>129</v>
-      </c>
+      <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="8" t="s">
-        <v>130</v>
-      </c>
+      <c r="D37" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UserGame controller/view changes to user new UserGamesViewModel
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="128">
   <si>
     <t>Status</t>
   </si>
@@ -410,16 +410,10 @@
     <t>NEXT</t>
   </si>
   <si>
-    <t>REVISIT</t>
-  </si>
-  <si>
     <t>Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. -&gt; Viewmodel UsersByGame</t>
   </si>
   <si>
     <t xml:space="preserve">Ties to item below. Note: Should also be able to show all games subscribed -&gt; Will require a view model. </t>
-  </si>
-  <si>
-    <t>Change the UserGame table to use the userid, and update the controllers. Then create viewmodel that shows the e-mail rather than the userid, and update the views.</t>
   </si>
 </sst>
 </file>
@@ -556,7 +550,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -573,6 +567,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1338,7 +1333,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1546,7 @@
         <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,22 +1560,20 @@
         <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>129</v>
-      </c>
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
WarmachineGame m/v/c stubbed in
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="129">
   <si>
     <t>Status</t>
   </si>
@@ -407,13 +407,16 @@
     <t xml:space="preserve">Refactored this to use a custom Html Helper for images. </t>
   </si>
   <si>
-    <t>NEXT</t>
-  </si>
-  <si>
     <t>Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. -&gt; Viewmodel UsersByGame</t>
   </si>
   <si>
     <t xml:space="preserve">Ties to item below. Note: Should also be able to show all games subscribed -&gt; Will require a view model. </t>
+  </si>
+  <si>
+    <t>NEXT 1</t>
+  </si>
+  <si>
+    <t>NEXT 2</t>
   </si>
 </sst>
 </file>
@@ -1332,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,10 +1546,10 @@
         <v>84</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,10 +1560,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" t="s">
         <v>125</v>
-      </c>
-      <c r="D19" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Warmachine game entry - userid as hidden field
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\CSharp\StatsMachine\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Code\CSharp\StatsMachine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="M-0.5" sheetId="4" r:id="rId1"/>
-    <sheet name="M0 - Account Mgmt" sheetId="5" r:id="rId2"/>
-    <sheet name="M-1 Tasks" sheetId="1" r:id="rId3"/>
+    <sheet name="M-1 Tasks" sheetId="1" r:id="rId1"/>
+    <sheet name="M-0.5" sheetId="4" r:id="rId2"/>
+    <sheet name="M0 - Account Mgmt" sheetId="5" r:id="rId3"/>
     <sheet name="M1 - Game Data" sheetId="6" r:id="rId4"/>
     <sheet name="Links" sheetId="2" r:id="rId5"/>
     <sheet name="Notes" sheetId="3" r:id="rId6"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="148">
   <si>
     <t>Status</t>
   </si>
@@ -329,9 +329,6 @@
     <t>UserGame Controller</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t xml:space="preserve">Logos live on webserver and are loaded based on a path string derived from a stored faction db entry. </t>
   </si>
   <si>
@@ -453,6 +450,30 @@
   </si>
   <si>
     <t xml:space="preserve">Game opponents are displayed as hyperlinks if the user exists. </t>
+  </si>
+  <si>
+    <t>User can edit data for their own game.</t>
+  </si>
+  <si>
+    <t>Change to View Model that shows names. Also need to add filter. (Route? )</t>
+  </si>
+  <si>
+    <t>Admin can edit a game entry</t>
+  </si>
+  <si>
+    <t>Admin can delete a game entry</t>
+  </si>
+  <si>
+    <t>User can delete their own game entry</t>
+  </si>
+  <si>
+    <t>Need to restrict this to the owning user</t>
+  </si>
+  <si>
+    <t>Expand/Collapse non-required fields in the entry form.</t>
+  </si>
+  <si>
+    <t>Ability to add army list field to WarmachineGame model</t>
   </si>
 </sst>
 </file>
@@ -894,6 +915,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1064,12 +1357,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1398,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,7 +1420,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1143,7 +1436,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -1154,7 +1447,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -1165,10 +1458,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
         <v>103</v>
-      </c>
-      <c r="B8" t="s">
-        <v>104</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>18</v>
@@ -1176,7 +1469,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
         <v>84</v>
@@ -1187,16 +1480,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
         <v>119</v>
       </c>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1268,7 +1561,7 @@
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,10 +1572,10 @@
         <v>84</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,10 +1586,10 @@
         <v>84</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1323,7 +1616,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,27 +1632,27 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
         <v>110</v>
       </c>
-      <c r="B23" t="s">
-        <v>111</v>
-      </c>
       <c r="C23" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>117</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1431,7 +1724,7 @@
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1442,7 +1735,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1455,7 +1748,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
         <v>87</v>
@@ -1466,18 +1759,18 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
         <v>108</v>
-      </c>
-      <c r="B35" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
         <v>113</v>
-      </c>
-      <c r="B36" t="s">
-        <v>114</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>18</v>
@@ -1495,283 +1788,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="62.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -1797,6 +1818,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>78</v>
@@ -1813,7 +1850,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>18</v>
@@ -1821,75 +1858,107 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>99</v>
+        <v>128</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>133</v>
       </c>
-      <c r="B20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B23" t="s">
         <v>134</v>
       </c>
-      <c r="B21" t="s">
-        <v>135</v>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Game list view model with userid-to-username matching
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="M-1 Tasks" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="150">
   <si>
     <t>Status</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Should to filter by game (Warmachine by default). Also think about how to store/retrieve score summary data. -&gt; Viewmodel UsersByGame</t>
   </si>
   <si>
-    <t xml:space="preserve">Ties to item below. Note: Should also be able to show all games subscribed -&gt; Will require a view model. </t>
-  </si>
-  <si>
     <t>NEXT 1</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>Game opponents are pulled from database if they exist</t>
   </si>
   <si>
-    <t xml:space="preserve">Game opponents are displayed as hyperlinks if the user exists. </t>
-  </si>
-  <si>
     <t>User can edit data for their own game.</t>
   </si>
   <si>
@@ -474,6 +468,18 @@
   </si>
   <si>
     <t>Ability to add army list field to WarmachineGame model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game entries have dates, and dates can be edited. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game opponents are displayed as hyperlinks to userid if the user exists. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ties to item below. Note: Should also be able to show all games subscribed -&gt; Will require a view model.    CREATE A USER PROFILE PAGE THAT USES INFO BOX FOR ANY USER. </t>
+  </si>
+  <si>
+    <t>Link to user profile page once created. (See M0)</t>
   </si>
 </sst>
 </file>
@@ -1361,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,10 +1578,10 @@
         <v>84</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,7 +1592,7 @@
         <v>84</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
         <v>123</v>
@@ -1792,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,7 +1826,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>18</v>
@@ -1828,7 +1834,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>18</v>
@@ -1850,7 +1856,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>18</v>
@@ -1858,7 +1864,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>18</v>
@@ -1866,46 +1872,49 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>18</v>
@@ -1913,12 +1922,21 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>147</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1937,32 +1955,33 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" t="s">
         <v>133</v>
-      </c>
-      <c r="B23" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Warmachine games - list all or by user. None faction added
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="M-1 Tasks" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="152">
   <si>
     <t>Status</t>
   </si>
@@ -419,9 +419,6 @@
     <t>User can view all games player by all users - Filtered by game</t>
   </si>
   <si>
-    <t>User can view all game entried by ANOTHER user</t>
-  </si>
-  <si>
     <t>UserInfoBox contains game stats totals (wins, losses, etc.)</t>
   </si>
   <si>
@@ -479,7 +476,29 @@
     <t xml:space="preserve">Ties to item below. Note: Should also be able to show all games subscribed -&gt; Will require a view model.    CREATE A USER PROFILE PAGE THAT USES INFO BOX FOR ANY USER. </t>
   </si>
   <si>
-    <t>Link to user profile page once created. (See M0)</t>
+    <t>Need to restrict this to the owning user -&gt; 1) Edit only on own controller (2) Compare ids in controller</t>
+  </si>
+  <si>
+    <t>User can view all game entries by ANOTHER user</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Link to profile page. --- Techincally done, but need way to pass a userid. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DO USER PROFILE VIEW NEXT</t>
+    </r>
+  </si>
+  <si>
+    <t>FIX THIS! SERIOUSLY! Will need data migration</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,7 +1600,7 @@
         <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1798,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,7 +1845,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>18</v>
@@ -1834,7 +1853,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>18</v>
@@ -1872,49 +1891,52 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
         <v>142</v>
-      </c>
-      <c r="D11" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>128</v>
       </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>18</v>
@@ -1922,7 +1944,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>18</v>
@@ -1930,13 +1952,16 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,28 +1980,28 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
         <v>132</v>
-      </c>
-      <c r="B23" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>